<commit_message>
local change in data
</commit_message>
<xml_diff>
--- a/Testing Dataset.xlsx
+++ b/Testing Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaom\OneDrive\Desktop\Github Folder\Alcohol-Consumption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ECE3F8-74AC-4478-BCB3-C23FB7F624DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B543BCE4-6FCB-4AC1-8E47-6045E7AF7632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3936" yWindow="552" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -381,9 +381,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -493,6 +495,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>